<commit_message>
mise a jour pour stocker les donnees dans factures.xlsx
</commit_message>
<xml_diff>
--- a/data/Factures.xlsx
+++ b/data/Factures.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A16"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,6 +439,46 @@
           <t>numero_facture</t>
         </is>
       </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>code_client</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>nom_client</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>total_ht</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>remise_fcfa</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>taux_remise</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>tva</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>total_ttc</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -446,6 +486,14 @@
           <t>F0001</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -453,6 +501,14 @@
           <t>F0002</t>
         </is>
       </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -460,6 +516,14 @@
           <t>F0003</t>
         </is>
       </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -467,6 +531,14 @@
           <t>F0004</t>
         </is>
       </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -474,6 +546,14 @@
           <t>F0005</t>
         </is>
       </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -481,6 +561,14 @@
           <t>F0006</t>
         </is>
       </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -488,6 +576,14 @@
           <t>F0007</t>
         </is>
       </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -495,6 +591,14 @@
           <t>F0008</t>
         </is>
       </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -502,6 +606,14 @@
           <t>F0009</t>
         </is>
       </c>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -509,6 +621,14 @@
           <t>F0010</t>
         </is>
       </c>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -516,6 +636,14 @@
           <t>F0011</t>
         </is>
       </c>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -523,6 +651,14 @@
           <t>F0012</t>
         </is>
       </c>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -530,6 +666,14 @@
           <t>F0013</t>
         </is>
       </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -537,12 +681,65 @@
           <t>F0014</t>
         </is>
       </c>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
           <t>F0015</t>
         </is>
+      </c>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>F0016</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>C00003</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Florent b</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>20/07/2025</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>2380000</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" t="n">
+        <v>428400</v>
+      </c>
+      <c r="I17" t="n">
+        <v>2808400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>